<commit_message>
Rancangan database Model News
</commit_message>
<xml_diff>
--- a/docs/Rancangan WBS.xlsx
+++ b/docs/Rancangan WBS.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8340"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="104">
   <si>
     <t>Requirement:</t>
   </si>
@@ -237,6 +237,105 @@
   </si>
   <si>
     <t>Frontend</t>
+  </si>
+  <si>
+    <t>users</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>nim</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>auth_level</t>
+  </si>
+  <si>
+    <t>beasiswa</t>
+  </si>
+  <si>
+    <t>kategori</t>
+  </si>
+  <si>
+    <t>creation date(otomatis)</t>
+  </si>
+  <si>
+    <t>update date(otomatis)</t>
+  </si>
+  <si>
+    <t>DATABASE</t>
+  </si>
+  <si>
+    <t>beasiswa_content</t>
+  </si>
+  <si>
+    <t>beasiswa_id</t>
+  </si>
+  <si>
+    <t>sumber</t>
+  </si>
+  <si>
+    <t>jumlah</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>content</t>
+  </si>
+  <si>
+    <t>news</t>
+  </si>
+  <si>
+    <t>news_content</t>
+  </si>
+  <si>
+    <t>news_id</t>
+  </si>
+  <si>
+    <t>ukm</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>ukm_content</t>
+  </si>
+  <si>
+    <t>header_pic</t>
+  </si>
+  <si>
+    <t>ukm_id</t>
+  </si>
+  <si>
+    <t>event</t>
+  </si>
+  <si>
+    <t>deadline_date</t>
+  </si>
+  <si>
+    <t>creation_date(otomatis)</t>
+  </si>
+  <si>
+    <t>update_date(otomatis)</t>
+  </si>
+  <si>
+    <t>tempat</t>
+  </si>
+  <si>
+    <t>event_date</t>
+  </si>
+  <si>
+    <t>event_content</t>
+  </si>
+  <si>
+    <t>event_id</t>
   </si>
 </sst>
 </file>
@@ -849,10 +948,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:N45"/>
+  <dimension ref="A2:X45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -864,10 +963,19 @@
     <col min="5" max="5" width="38.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.140625" style="3"/>
     <col min="7" max="7" width="7.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="3"/>
+    <col min="8" max="15" width="9.140625" style="3"/>
+    <col min="16" max="17" width="31.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="22.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="31.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="31.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="18.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="25" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -875,8 +983,11 @@
       <c r="D2" s="4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P2" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
@@ -914,8 +1025,35 @@
         <v>42478</v>
       </c>
       <c r="N3" s="26"/>
-    </row>
-    <row r="4" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P3" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q3" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="R3" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="S3" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="T3" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="U3" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="V3" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="W3" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="X3" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="27" t="s">
         <v>3</v>
       </c>
@@ -937,8 +1075,35 @@
       <c r="L4" s="23"/>
       <c r="M4" s="23"/>
       <c r="N4" s="26"/>
-    </row>
-    <row r="5" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P4" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="T4" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="U4" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="V4" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="W4" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="X4" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="28"/>
       <c r="B5" s="8" t="s">
         <v>7</v>
@@ -958,8 +1123,35 @@
       <c r="L5" s="25"/>
       <c r="M5" s="25"/>
       <c r="N5" s="26"/>
-    </row>
-    <row r="6" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P5" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q5" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="R5" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="S5" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="T5" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="U5" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="V5" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="W5" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="X5" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>17</v>
       </c>
@@ -979,8 +1171,35 @@
       <c r="L6" s="23"/>
       <c r="M6" s="23"/>
       <c r="N6" s="26"/>
-    </row>
-    <row r="7" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P6" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q6" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="R6" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="S6" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="T6" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="U6" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="V6" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="W6" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="X6" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>2</v>
       </c>
@@ -1000,8 +1219,32 @@
       <c r="L7" s="23"/>
       <c r="M7" s="23"/>
       <c r="N7" s="26"/>
-    </row>
-    <row r="8" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P7" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q7" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="R7" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="S7" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="T7" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="V7" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="W7" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="X7" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>8</v>
       </c>
@@ -1023,8 +1266,17 @@
       <c r="L8" s="23"/>
       <c r="M8" s="23"/>
       <c r="N8" s="26"/>
-    </row>
-    <row r="9" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P8" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q8" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="W8" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>22</v>
       </c>
@@ -1046,8 +1298,17 @@
       <c r="L9" s="23"/>
       <c r="M9" s="23"/>
       <c r="N9" s="26"/>
-    </row>
-    <row r="10" spans="1:14" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P9" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q9" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="W9" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
         <v>15</v>
       </c>
@@ -1069,8 +1330,17 @@
       <c r="L10" s="23"/>
       <c r="M10" s="23"/>
       <c r="N10" s="26"/>
-    </row>
-    <row r="11" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P10" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q10" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="W10" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D11" s="23" t="s">
         <v>69</v>
       </c>
@@ -1086,8 +1356,14 @@
       <c r="L11" s="23"/>
       <c r="M11" s="23"/>
       <c r="N11" s="26"/>
-    </row>
-    <row r="12" spans="1:14" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q11" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="W11" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>10</v>
       </c>
@@ -1107,7 +1383,7 @@
       <c r="M12" s="23"/>
       <c r="N12" s="26"/>
     </row>
-    <row r="13" spans="1:14" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:24" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="14" t="s">
         <v>5</v>
       </c>
@@ -1130,7 +1406,7 @@
       <c r="M13" s="23"/>
       <c r="N13" s="26"/>
     </row>
-    <row r="14" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>11</v>
       </c>
@@ -1151,7 +1427,7 @@
       <c r="M14" s="23"/>
       <c r="N14" s="26"/>
     </row>
-    <row r="15" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
         <v>12</v>
       </c>
@@ -1174,7 +1450,7 @@
       <c r="M15" s="23"/>
       <c r="N15" s="26"/>
     </row>
-    <row r="16" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="18"/>
       <c r="B16" s="19" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
wbs sama migration user sama news
</commit_message>
<xml_diff>
--- a/docs/Rancangan WBS.xlsx
+++ b/docs/Rancangan WBS.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\SiTiOne\docs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8340"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="104">
   <si>
     <t>Requirement:</t>
   </si>
@@ -245,9 +240,6 @@
     <t>id</t>
   </si>
   <si>
-    <t>nim</t>
-  </si>
-  <si>
     <t>password</t>
   </si>
   <si>
@@ -336,13 +328,16 @@
   </si>
   <si>
     <t>event_id</t>
+  </si>
+  <si>
+    <t>images</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -728,7 +723,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -763,7 +758,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -940,21 +935,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:X45"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A2:Y45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="T5" sqref="T5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="19.5" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="16.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.28515625" style="3" bestFit="1" customWidth="1"/>
@@ -975,7 +970,7 @@
     <col min="25" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:24" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25" ht="19.5" customHeight="1" thickBot="1">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -984,10 +979,10 @@
         <v>1</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" ht="19.5" customHeight="1" thickBot="1">
       <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
@@ -1029,31 +1024,34 @@
         <v>71</v>
       </c>
       <c r="Q3" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="R3" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="S3" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="T3" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="T3" s="4" t="s">
-        <v>89</v>
-      </c>
       <c r="U3" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="V3" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="W3" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="X3" s="4" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="Y3" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" ht="19.5" customHeight="1">
       <c r="A4" s="27" t="s">
         <v>3</v>
       </c>
@@ -1082,28 +1080,31 @@
         <v>72</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="S4" s="3" t="s">
         <v>72</v>
       </c>
       <c r="T4" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="U4" s="3" t="s">
         <v>72</v>
       </c>
       <c r="V4" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="W4" s="3" t="s">
         <v>72</v>
       </c>
       <c r="X4" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+      <c r="Y4" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" ht="19.5" customHeight="1">
       <c r="A5" s="28"/>
       <c r="B5" s="8" t="s">
         <v>7</v>
@@ -1124,34 +1125,37 @@
       <c r="M5" s="25"/>
       <c r="N5" s="26"/>
       <c r="P5" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="R5" s="3" t="s">
         <v>72</v>
       </c>
       <c r="S5" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="T5" s="3" t="s">
         <v>72</v>
       </c>
       <c r="U5" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="V5" s="3" t="s">
         <v>72</v>
       </c>
       <c r="W5" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="X5" s="3" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="6" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Y5" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" ht="19.5" customHeight="1">
       <c r="A6" s="9" t="s">
         <v>17</v>
       </c>
@@ -1172,34 +1176,34 @@
       <c r="M6" s="23"/>
       <c r="N6" s="26"/>
       <c r="P6" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="R6" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="S6" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="T6" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="U6" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="V6" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="W6" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="X6" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="7" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" ht="19.5" customHeight="1">
       <c r="A7" s="9" t="s">
         <v>2</v>
       </c>
@@ -1220,31 +1224,31 @@
       <c r="M7" s="23"/>
       <c r="N7" s="26"/>
       <c r="P7" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="Q7" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="R7" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="S7" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="T7" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="V7" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="W7" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="X7" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="8" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" ht="19.5" customHeight="1">
       <c r="A8" s="9" t="s">
         <v>8</v>
       </c>
@@ -1267,16 +1271,16 @@
       <c r="M8" s="23"/>
       <c r="N8" s="26"/>
       <c r="P8" s="3" t="s">
-        <v>76</v>
+        <v>98</v>
       </c>
       <c r="Q8" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="W8" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" ht="19.5" customHeight="1">
       <c r="A9" s="10" t="s">
         <v>22</v>
       </c>
@@ -1299,16 +1303,16 @@
       <c r="M9" s="23"/>
       <c r="N9" s="26"/>
       <c r="P9" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="Q9" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="W9" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="10" spans="1:24" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" ht="19.5" customHeight="1" thickBot="1">
       <c r="A10" s="12" t="s">
         <v>15</v>
       </c>
@@ -1330,17 +1334,14 @@
       <c r="L10" s="23"/>
       <c r="M10" s="23"/>
       <c r="N10" s="26"/>
-      <c r="P10" s="3" t="s">
-        <v>98</v>
-      </c>
       <c r="Q10" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="W10" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="11" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" ht="19.5" customHeight="1">
       <c r="D11" s="23" t="s">
         <v>69</v>
       </c>
@@ -1357,13 +1358,13 @@
       <c r="M11" s="23"/>
       <c r="N11" s="26"/>
       <c r="Q11" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="W11" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="12" spans="1:24" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" ht="19.5" customHeight="1" thickBot="1">
       <c r="A12" s="4" t="s">
         <v>10</v>
       </c>
@@ -1383,7 +1384,7 @@
       <c r="M12" s="23"/>
       <c r="N12" s="26"/>
     </row>
-    <row r="13" spans="1:24" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:25" ht="19.5" customHeight="1" thickBot="1">
       <c r="A13" s="14" t="s">
         <v>5</v>
       </c>
@@ -1406,7 +1407,7 @@
       <c r="M13" s="23"/>
       <c r="N13" s="26"/>
     </row>
-    <row r="14" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" ht="19.5" customHeight="1">
       <c r="A14" s="16" t="s">
         <v>11</v>
       </c>
@@ -1427,7 +1428,7 @@
       <c r="M14" s="23"/>
       <c r="N14" s="26"/>
     </row>
-    <row r="15" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" ht="19.5" customHeight="1">
       <c r="A15" s="18" t="s">
         <v>12</v>
       </c>
@@ -1450,7 +1451,7 @@
       <c r="M15" s="23"/>
       <c r="N15" s="26"/>
     </row>
-    <row r="16" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" ht="19.5" customHeight="1">
       <c r="A16" s="18"/>
       <c r="B16" s="19" t="s">
         <v>13</v>
@@ -1471,7 +1472,7 @@
       <c r="M16" s="23"/>
       <c r="N16" s="26"/>
     </row>
-    <row r="17" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" ht="19.5" customHeight="1">
       <c r="A17" s="18"/>
       <c r="B17" s="19" t="s">
         <v>21</v>
@@ -1492,7 +1493,7 @@
       <c r="M17" s="23"/>
       <c r="N17" s="26"/>
     </row>
-    <row r="18" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" ht="19.5" customHeight="1">
       <c r="A18" s="18" t="s">
         <v>16</v>
       </c>
@@ -1515,7 +1516,7 @@
       <c r="M18" s="23"/>
       <c r="N18" s="26"/>
     </row>
-    <row r="19" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" ht="19.5" customHeight="1">
       <c r="A19" s="18"/>
       <c r="B19" s="19" t="s">
         <v>18</v>
@@ -1536,7 +1537,7 @@
       <c r="M19" s="23"/>
       <c r="N19" s="26"/>
     </row>
-    <row r="20" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" ht="19.5" customHeight="1">
       <c r="A20" s="18"/>
       <c r="B20" s="19" t="s">
         <v>20</v>
@@ -1557,7 +1558,7 @@
       <c r="M20" s="23"/>
       <c r="N20" s="26"/>
     </row>
-    <row r="21" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" ht="19.5" customHeight="1">
       <c r="A21" s="18" t="s">
         <v>24</v>
       </c>
@@ -1580,7 +1581,7 @@
       <c r="M21" s="23"/>
       <c r="N21" s="26"/>
     </row>
-    <row r="22" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" ht="19.5" customHeight="1">
       <c r="A22" s="18"/>
       <c r="B22" s="19" t="s">
         <v>26</v>
@@ -1601,7 +1602,7 @@
       <c r="M22" s="23"/>
       <c r="N22" s="26"/>
     </row>
-    <row r="23" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" ht="19.5" customHeight="1">
       <c r="A23" s="18"/>
       <c r="B23" s="19" t="s">
         <v>27</v>
@@ -1622,7 +1623,7 @@
       <c r="M23" s="23"/>
       <c r="N23" s="26"/>
     </row>
-    <row r="24" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" ht="19.5" customHeight="1">
       <c r="A24" s="18" t="s">
         <v>28</v>
       </c>
@@ -1645,7 +1646,7 @@
       <c r="M24" s="23"/>
       <c r="N24" s="26"/>
     </row>
-    <row r="25" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" ht="19.5" customHeight="1">
       <c r="A25" s="18"/>
       <c r="B25" s="19" t="s">
         <v>30</v>
@@ -1666,7 +1667,7 @@
       <c r="M25" s="23"/>
       <c r="N25" s="26"/>
     </row>
-    <row r="26" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" ht="19.5" customHeight="1">
       <c r="A26" s="18"/>
       <c r="B26" s="19" t="s">
         <v>31</v>
@@ -1687,7 +1688,7 @@
       <c r="M26" s="23"/>
       <c r="N26" s="26"/>
     </row>
-    <row r="27" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" ht="19.5" customHeight="1">
       <c r="A27" s="18" t="s">
         <v>32</v>
       </c>
@@ -1710,7 +1711,7 @@
       <c r="M27" s="23"/>
       <c r="N27" s="26"/>
     </row>
-    <row r="28" spans="1:14" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" ht="19.5" customHeight="1" thickBot="1">
       <c r="A28" s="20" t="s">
         <v>34</v>
       </c>
@@ -1733,7 +1734,7 @@
       <c r="M28" s="23"/>
       <c r="N28" s="26"/>
     </row>
-    <row r="29" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" ht="19.5" customHeight="1">
       <c r="D29" s="23" t="s">
         <v>70</v>
       </c>
@@ -1750,7 +1751,7 @@
       <c r="M29" s="23"/>
       <c r="N29" s="26"/>
     </row>
-    <row r="30" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" ht="19.5" customHeight="1">
       <c r="D30" s="23" t="s">
         <v>70</v>
       </c>
@@ -1767,7 +1768,7 @@
       <c r="M30" s="23"/>
       <c r="N30" s="26"/>
     </row>
-    <row r="31" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" ht="19.5" customHeight="1">
       <c r="D31" s="23" t="s">
         <v>69</v>
       </c>
@@ -1784,7 +1785,7 @@
       <c r="M31" s="23"/>
       <c r="N31" s="26"/>
     </row>
-    <row r="32" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" ht="19.5" customHeight="1">
       <c r="D32" s="23" t="s">
         <v>69</v>
       </c>
@@ -1801,7 +1802,7 @@
       <c r="M32" s="23"/>
       <c r="N32" s="26"/>
     </row>
-    <row r="33" spans="4:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:14" ht="19.5" customHeight="1">
       <c r="D33" s="23" t="s">
         <v>69</v>
       </c>
@@ -1818,7 +1819,7 @@
       <c r="M33" s="23"/>
       <c r="N33" s="26"/>
     </row>
-    <row r="34" spans="4:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:14" ht="19.5" customHeight="1">
       <c r="D34" s="23" t="s">
         <v>69</v>
       </c>
@@ -1835,7 +1836,7 @@
       <c r="M34" s="23"/>
       <c r="N34" s="26"/>
     </row>
-    <row r="35" spans="4:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:14" ht="19.5" customHeight="1">
       <c r="D35" s="23" t="s">
         <v>69</v>
       </c>
@@ -1852,7 +1853,7 @@
       <c r="M35" s="23"/>
       <c r="N35" s="26"/>
     </row>
-    <row r="36" spans="4:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:14" ht="19.5" customHeight="1">
       <c r="D36" s="23" t="s">
         <v>70</v>
       </c>
@@ -1869,7 +1870,7 @@
       <c r="M36" s="23"/>
       <c r="N36" s="26"/>
     </row>
-    <row r="37" spans="4:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:14" ht="19.5" customHeight="1">
       <c r="D37" s="23" t="s">
         <v>70</v>
       </c>
@@ -1886,7 +1887,7 @@
       <c r="M37" s="23"/>
       <c r="N37" s="26"/>
     </row>
-    <row r="38" spans="4:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:14" ht="19.5" customHeight="1">
       <c r="D38" s="23" t="s">
         <v>70</v>
       </c>
@@ -1903,7 +1904,7 @@
       <c r="M38" s="23"/>
       <c r="N38" s="26"/>
     </row>
-    <row r="39" spans="4:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:14" ht="19.5" customHeight="1">
       <c r="D39" s="23" t="s">
         <v>70</v>
       </c>
@@ -1920,7 +1921,7 @@
       <c r="M39" s="23"/>
       <c r="N39" s="26"/>
     </row>
-    <row r="40" spans="4:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:14" ht="19.5" customHeight="1">
       <c r="D40" s="23" t="s">
         <v>70</v>
       </c>
@@ -1937,7 +1938,7 @@
       <c r="M40" s="23"/>
       <c r="N40" s="26"/>
     </row>
-    <row r="41" spans="4:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:14" ht="19.5" customHeight="1">
       <c r="D41" s="23" t="s">
         <v>69</v>
       </c>
@@ -1954,7 +1955,7 @@
       <c r="M41" s="23"/>
       <c r="N41" s="26"/>
     </row>
-    <row r="42" spans="4:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="4:14" ht="19.5" customHeight="1">
       <c r="D42" s="23" t="s">
         <v>69</v>
       </c>
@@ -1971,7 +1972,7 @@
       <c r="M42" s="23"/>
       <c r="N42" s="26"/>
     </row>
-    <row r="43" spans="4:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="4:14" ht="19.5" customHeight="1">
       <c r="D43" s="23" t="s">
         <v>69</v>
       </c>
@@ -1988,7 +1989,7 @@
       <c r="M43" s="23"/>
       <c r="N43" s="26"/>
     </row>
-    <row r="44" spans="4:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="4:14" ht="19.5" customHeight="1">
       <c r="D44" s="23" t="s">
         <v>69</v>
       </c>
@@ -2005,7 +2006,7 @@
       <c r="M44" s="23"/>
       <c r="N44" s="26"/>
     </row>
-    <row r="45" spans="4:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="4:14" ht="19.5" customHeight="1">
       <c r="D45" s="23" t="s">
         <v>69</v>
       </c>
@@ -2027,6 +2028,6 @@
     <mergeCell ref="A4:A5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
edit migration users (tambah boolean is_aktif)
</commit_message>
<xml_diff>
--- a/docs/Rancangan WBS.xlsx
+++ b/docs/Rancangan WBS.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="105">
   <si>
     <t>Requirement:</t>
   </si>
@@ -331,6 +331,9 @@
   </si>
   <si>
     <t>images</t>
+  </si>
+  <si>
+    <t>is_aktif</t>
   </si>
 </sst>
 </file>
@@ -935,7 +938,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -945,8 +948,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:Y45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="T5" sqref="T5"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" customHeight="1"/>
@@ -1334,6 +1337,9 @@
       <c r="L10" s="23"/>
       <c r="M10" s="23"/>
       <c r="N10" s="26"/>
+      <c r="P10" s="3" t="s">
+        <v>104</v>
+      </c>
       <c r="Q10" s="3" t="s">
         <v>97</v>
       </c>

</xml_diff>

<commit_message>
edit wbs + controller news(edit)
</commit_message>
<xml_diff>
--- a/docs/Rancangan WBS.xlsx
+++ b/docs/Rancangan WBS.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="105">
   <si>
     <t>Requirement:</t>
   </si>
@@ -336,6 +336,9 @@
   </si>
   <si>
     <t>status</t>
+  </si>
+  <si>
+    <t>News Controller - edit</t>
   </si>
 </sst>
 </file>
@@ -948,10 +951,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:X45"/>
+  <dimension ref="A2:X46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" topLeftCell="C31" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2021,6 +2024,22 @@
       <c r="M45" s="23"/>
       <c r="N45" s="26"/>
     </row>
+    <row r="46" spans="4:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D46" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="E46" s="23" t="s">
+        <v>104</v>
+      </c>
+      <c r="F46" s="23"/>
+      <c r="G46" s="23"/>
+      <c r="H46" s="23"/>
+      <c r="I46" s="25"/>
+      <c r="J46" s="25"/>
+      <c r="K46" s="25"/>
+      <c r="L46" s="25"/>
+      <c r="M46" s="23"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A4:A5"/>

</xml_diff>